<commit_message>
deleting unused file and adding images
</commit_message>
<xml_diff>
--- a/Resources/contacts.xlsx
+++ b/Resources/contacts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d7cf462ad91b6727/Desktop/Project 2/Crowdfunding_ETL/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{BA862834-D96C-9D43-87C0-A2A9BCCC1B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B15F51FC-73CD-4051-8E96-2F52D0A03EC8}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{BA862834-D96C-9D43-87C0-A2A9BCCC1B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99619A1D-5C82-43C6-BAE3-B6F905FA57AE}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1395" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact_info" sheetId="2" r:id="rId1"/>
@@ -3078,7 +3078,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{D99AEA5C-4E65-4460-8A8E-AEBA7692B9ED}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{875444C5-EAE3-4C33-817B-579DE70E10D5}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">

</xml_diff>